<commit_message>
Updated script build_model.py with optimizer option and added new visualizations. 1. Added Adam optimizer to fitting the model. Usage of the optimizer allowed to train the model faster and use fewer minibatches. 2. Added new visualizations of doodles: grid with doodles and animated gifs. 3. Added script build_random_forest.py to compare nn with RF classification.
</commit_message>
<xml_diff>
--- a/analysis/hyperparameters_comparison.xlsx
+++ b/analysis/hyperparameters_comparison.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandraastakhova/Projects/Python/Quick Draw/quick-draw-image-recognition/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEE5191-27C1-3948-B16E-73FA05C88569}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F68D837-367C-5D40-9DD5-E26C6933AE25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1500" windowWidth="28240" windowHeight="17560" xr2:uid="{7776EE55-F732-E243-947B-1C2E89181C75}"/>
+    <workbookView xWindow="2320" yWindow="1600" windowWidth="28240" windowHeight="17560" activeTab="2" xr2:uid="{7776EE55-F732-E243-947B-1C2E89181C75}"/>
   </bookViews>
   <sheets>
-    <sheet name="Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Original dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Expanded dataset" sheetId="2" r:id="rId2"/>
+    <sheet name="Adam optimizer" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="hyperparameter_comparison" localSheetId="0">Parameters!$B$4:$K$14</definedName>
+    <definedName name="comparison_1557179772.093524" localSheetId="2">'Adam optimizer'!$B$4:$I$14</definedName>
+    <definedName name="hyperparameter_comparison" localSheetId="0">'Original dataset'!$B$4:$K$14</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +38,20 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{58768D16-446B-2C43-AEFF-3CEAED3B1F3B}" name="hyperparameter_comparison" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{12D849D9-0D93-2042-82CE-AA97A3155C30}" name="comparison_1557179772.093524" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10007" sourceFile="/Users/aleksandraastakhova/Projects/Python/Quick Draw/comparison_1557179772.093524.csv" thousands=" " comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" xr16:uid="{58768D16-446B-2C43-AEFF-3CEAED3B1F3B}" name="hyperparameter_comparison" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10007" sourceFile="/Users/aleksandraastakhova/Projects/Python/Quick Draw/hyperparameter_comparison.csv" thousands=" " tab="0" comma="1">
       <textFields count="9">
         <textField/>
@@ -54,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>test weight_decay: 0.0, dropout: 0.0</t>
   </si>
@@ -80,13 +96,19 @@
     <t>train weight_decay: 0.1, dropout: 0.0</t>
   </si>
   <si>
-    <t>Comparison of hyperparameters for the feed-forward neural network</t>
-  </si>
-  <si>
     <t>epochs</t>
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>Comparison of hyperparameters for the feed-forward neural network (lr = 0.03)</t>
+  </si>
+  <si>
+    <t>Comparison of hyperparameters for the feed-forward neural network (lr = 0.03, expanded dataset with rotated and flipped images)</t>
+  </si>
+  <si>
+    <t>Comparison of hyperparameters for the feed-forward neural network (lr = 0.03, expanded dataset with rotated and flipped images) with Adam optimizer and number of minibatches == 1000</t>
   </si>
 </sst>
 </file>
@@ -152,7 +174,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hyperparameter_comparison" connectionId="1" xr16:uid="{BA1644FB-2D55-3E41-9BFC-E3B5AE7525F5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hyperparameter_comparison" connectionId="2" xr16:uid="{BA1644FB-2D55-3E41-9BFC-E3B5AE7525F5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="comparison_1557179772.093524" connectionId="1" xr16:uid="{3BE52358-A770-7945-B8C3-771A99E8AA11}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -454,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EEA5C6-2C24-CC4D-93E9-0641633C0B89}">
   <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,15 +501,15 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -828,6 +854,640 @@
       </c>
       <c r="K14">
         <v>0.10142857142857099</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8339C909-F14C-2C4C-BA89-011C8338A229}">
+  <dimension ref="B2:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.5" customWidth="1"/>
+    <col min="7" max="8" width="31.33203125" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.81144444444444397</v>
+      </c>
+      <c r="G5">
+        <v>0.83311111111111102</v>
+      </c>
+      <c r="H5">
+        <v>0.80144444444444396</v>
+      </c>
+      <c r="I5">
+        <v>0.81565079365079296</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>0.84733333333333305</v>
+      </c>
+      <c r="E6">
+        <v>0.93088888888888799</v>
+      </c>
+      <c r="F6">
+        <v>0.84422222222222199</v>
+      </c>
+      <c r="G6">
+        <v>0.898126984126984</v>
+      </c>
+      <c r="H6">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="I6">
+        <v>0.87431746031746005</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0.84355555555555495</v>
+      </c>
+      <c r="E7">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="F7">
+        <v>0.83622222222222198</v>
+      </c>
+      <c r="G7">
+        <v>0.92280952380952297</v>
+      </c>
+      <c r="H7">
+        <v>0.83077777777777695</v>
+      </c>
+      <c r="I7">
+        <v>0.91007936507936504</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>0.84211111111111103</v>
+      </c>
+      <c r="E8">
+        <v>0.97466666666666602</v>
+      </c>
+      <c r="F8">
+        <v>0.83855555555555505</v>
+      </c>
+      <c r="G8">
+        <v>0.94658730158730098</v>
+      </c>
+      <c r="H8">
+        <v>0.82811111111111102</v>
+      </c>
+      <c r="I8">
+        <v>0.92312698412698402</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>0.82511111111111102</v>
+      </c>
+      <c r="E9">
+        <v>0.98295238095238002</v>
+      </c>
+      <c r="F9">
+        <v>0.83288888888888801</v>
+      </c>
+      <c r="G9">
+        <v>0.95223809523809499</v>
+      </c>
+      <c r="H9">
+        <v>0.83</v>
+      </c>
+      <c r="I9">
+        <v>0.94266666666666599</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>0.82822222222222197</v>
+      </c>
+      <c r="E10">
+        <v>0.98668253968253905</v>
+      </c>
+      <c r="F10">
+        <v>0.82955555555555505</v>
+      </c>
+      <c r="G10">
+        <v>0.96342857142857097</v>
+      </c>
+      <c r="H10">
+        <v>0.83155555555555505</v>
+      </c>
+      <c r="I10">
+        <v>0.95079365079364997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>70</v>
+      </c>
+      <c r="D11">
+        <v>0.82877777777777695</v>
+      </c>
+      <c r="E11">
+        <v>0.99574603174603105</v>
+      </c>
+      <c r="F11">
+        <v>0.83</v>
+      </c>
+      <c r="G11">
+        <v>0.97231746031746003</v>
+      </c>
+      <c r="H11">
+        <v>0.82211111111111101</v>
+      </c>
+      <c r="I11">
+        <v>0.949031746031746</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>0.822888888888888</v>
+      </c>
+      <c r="E12">
+        <v>0.96053968253968203</v>
+      </c>
+      <c r="F12">
+        <v>0.83088888888888801</v>
+      </c>
+      <c r="G12">
+        <v>0.97649206349206297</v>
+      </c>
+      <c r="H12">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="I12">
+        <v>0.96077777777777695</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>90</v>
+      </c>
+      <c r="D13">
+        <v>0.83277777777777695</v>
+      </c>
+      <c r="E13">
+        <v>0.99995238095238004</v>
+      </c>
+      <c r="F13">
+        <v>0.82177777777777705</v>
+      </c>
+      <c r="G13">
+        <v>0.97319047619047605</v>
+      </c>
+      <c r="H13">
+        <v>0.82877777777777695</v>
+      </c>
+      <c r="I13">
+        <v>0.96706349206349196</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>0.832666666666666</v>
+      </c>
+      <c r="E14">
+        <v>0.99996825396825395</v>
+      </c>
+      <c r="F14">
+        <v>0.82488888888888801</v>
+      </c>
+      <c r="G14">
+        <v>0.98312698412698396</v>
+      </c>
+      <c r="H14">
+        <v>0.82877777777777695</v>
+      </c>
+      <c r="I14">
+        <v>0.96949206349206296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81FE0B0-99D3-464F-8FF5-7416433A4FBB}">
+  <dimension ref="B2:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>0.83588888888888802</v>
+      </c>
+      <c r="E5">
+        <v>0.94531746031746</v>
+      </c>
+      <c r="F5">
+        <v>0.83155555555555505</v>
+      </c>
+      <c r="G5">
+        <v>0.91253968253968198</v>
+      </c>
+      <c r="H5">
+        <v>0.82655555555555504</v>
+      </c>
+      <c r="I5">
+        <v>0.89107936507936503</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>0.83411111111111103</v>
+      </c>
+      <c r="E6">
+        <v>0.96041269841269805</v>
+      </c>
+      <c r="F6">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="G6">
+        <v>0.93546031746031699</v>
+      </c>
+      <c r="H6">
+        <v>0.82444444444444398</v>
+      </c>
+      <c r="I6">
+        <v>0.91857142857142804</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0.83277777777777695</v>
+      </c>
+      <c r="E7">
+        <v>0.97846031746031703</v>
+      </c>
+      <c r="F7">
+        <v>0.82811111111111102</v>
+      </c>
+      <c r="G7">
+        <v>0.94363492063492005</v>
+      </c>
+      <c r="H7">
+        <v>0.82477777777777705</v>
+      </c>
+      <c r="I7">
+        <v>0.93326984126984103</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>0.83244444444444399</v>
+      </c>
+      <c r="E8">
+        <v>0.97396825396825304</v>
+      </c>
+      <c r="F8">
+        <v>0.83144444444444399</v>
+      </c>
+      <c r="G8">
+        <v>0.95376190476190403</v>
+      </c>
+      <c r="H8">
+        <v>0.82133333333333303</v>
+      </c>
+      <c r="I8">
+        <v>0.94420634920634905</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>0.83188888888888801</v>
+      </c>
+      <c r="E9">
+        <v>0.98161904761904695</v>
+      </c>
+      <c r="F9">
+        <v>0.82322222222222197</v>
+      </c>
+      <c r="G9">
+        <v>0.95171428571428496</v>
+      </c>
+      <c r="H9">
+        <v>0.82277777777777705</v>
+      </c>
+      <c r="I9">
+        <v>0.94993650793650797</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>0.82977777777777695</v>
+      </c>
+      <c r="E10">
+        <v>0.97912698412698396</v>
+      </c>
+      <c r="F10">
+        <v>0.823888888888888</v>
+      </c>
+      <c r="G10">
+        <v>0.95931746031746001</v>
+      </c>
+      <c r="H10">
+        <v>0.82155555555555504</v>
+      </c>
+      <c r="I10">
+        <v>0.95242857142857096</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>70</v>
+      </c>
+      <c r="D11">
+        <v>0.82933333333333303</v>
+      </c>
+      <c r="E11">
+        <v>0.98411111111111105</v>
+      </c>
+      <c r="F11">
+        <v>0.82555555555555504</v>
+      </c>
+      <c r="G11">
+        <v>0.96560317460317402</v>
+      </c>
+      <c r="H11">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="I11">
+        <v>0.95587301587301499</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>0.82411111111111102</v>
+      </c>
+      <c r="E12">
+        <v>0.98577777777777698</v>
+      </c>
+      <c r="F12">
+        <v>0.82566666666666599</v>
+      </c>
+      <c r="G12">
+        <v>0.96820634920634896</v>
+      </c>
+      <c r="H12">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="I12">
+        <v>0.95630158730158699</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>90</v>
+      </c>
+      <c r="D13">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="E13">
+        <v>0.98561904761904695</v>
+      </c>
+      <c r="F13">
+        <v>0.82322222222222197</v>
+      </c>
+      <c r="G13">
+        <v>0.96276190476190404</v>
+      </c>
+      <c r="H13">
+        <v>0.81722222222222196</v>
+      </c>
+      <c r="I13">
+        <v>0.95950793650793598</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>0.83322222222222198</v>
+      </c>
+      <c r="E14">
+        <v>0.99012698412698397</v>
+      </c>
+      <c r="F14">
+        <v>0.81655555555555503</v>
+      </c>
+      <c r="G14">
+        <v>0.96915873015873</v>
+      </c>
+      <c r="H14">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="I14">
+        <v>0.96379365079364998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added image preprocessing: 1. Updated image_utils.py: added function crop_image to crop image to center and resize the image to 28x28 to be processed by the model. 2. Updated image_utils.py: added function normalize_image to normalize image colors after cropping and resizing the image before passing to the model. 3. Updated run.py of the web app: added preprocessing of the images passed from the main page.
</commit_message>
<xml_diff>
--- a/analysis/hyperparameters_comparison.xlsx
+++ b/analysis/hyperparameters_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandraastakhova/Projects/Python/Quick Draw/quick-draw-image-recognition/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F68D837-367C-5D40-9DD5-E26C6933AE25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2B8DFB-B214-AE46-B5CD-60E446049B0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="1600" windowWidth="28240" windowHeight="17560" activeTab="2" xr2:uid="{7776EE55-F732-E243-947B-1C2E89181C75}"/>
   </bookViews>
@@ -20,6 +20,8 @@
   <definedNames>
     <definedName name="comparison_1557179772.093524" localSheetId="2">'Adam optimizer'!$B$4:$I$14</definedName>
     <definedName name="hyperparameter_comparison" localSheetId="0">'Original dataset'!$B$4:$K$14</definedName>
+    <definedName name="learning_curve_adam_batch_norm" localSheetId="2">'Adam optimizer'!$J$4:$K$14</definedName>
+    <definedName name="learning_curve_adam_batch_norm_7000" localSheetId="2">'Adam optimizer'!$L$4:$M$14</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -66,11 +68,29 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" xr16:uid="{271E221C-F4AB-E244-B1AF-B9CEDBEFB65D}" name="learning_curve_adam_batch_norm" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10007" sourceFile="/Users/aleksandraastakhova/Projects/Python/Quick Draw/learning_curve_adam_batch_norm.csv" thousands=" " tab="0" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" xr16:uid="{AD48D861-32E6-F54D-AEB1-B3E184D14A53}" name="learning_curve_adam_batch_norm_7000" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10007" sourceFile="/Users/aleksandraastakhova/Projects/Python/Quick Draw/learning_curve_adam_batch_norm_7000.csv" thousands=" " tab="0" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>test weight_decay: 0.0, dropout: 0.0</t>
   </si>
@@ -105,10 +125,22 @@
     <t>Comparison of hyperparameters for the feed-forward neural network (lr = 0.03)</t>
   </si>
   <si>
-    <t>Comparison of hyperparameters for the feed-forward neural network (lr = 0.03, expanded dataset with rotated and flipped images)</t>
+    <t>Comparison of hyperparameters for the feed-forward neural network (lr = 0.03, expanded dataset with rotated and flipped images) with Adam optimizer and number of minibatches == 1000</t>
   </si>
   <si>
-    <t>Comparison of hyperparameters for the feed-forward neural network (lr = 0.03, expanded dataset with rotated and flipped images) with Adam optimizer and number of minibatches == 1000</t>
+    <t>train batch norm weight_decay: 0.0, dropout: 0.0</t>
+  </si>
+  <si>
+    <t>test batch norm weight_decay: 0.0, dropout: 0.0</t>
+  </si>
+  <si>
+    <t>Comparison of hyperparameters for the feed-forward neural network (lr = 0.03, expanded dataset with rotated and flipped images, minibatches = 7000)</t>
+  </si>
+  <si>
+    <t>train batch norm weight_decay: 0.0, dropout: 0.0 mini batches = 7000</t>
+  </si>
+  <si>
+    <t>test batch norm weight_decay: 0.0, dropout: 0.0, mini batches = 7000</t>
   </si>
 </sst>
 </file>
@@ -178,7 +210,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="learning_curve_adam_batch_norm_7000" connectionId="4" xr16:uid="{17E34221-FBAE-184A-930B-412F0C2EF5F0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="comparison_1557179772.093524" connectionId="1" xr16:uid="{3BE52358-A770-7945-B8C3-771A99E8AA11}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="learning_curve_adam_batch_norm" connectionId="3" xr16:uid="{B3314429-B1B6-BE45-AB91-D2B05C6A27EF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,10 +903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8339C909-F14C-2C4C-BA89-011C8338A229}">
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,14 +919,16 @@
     <col min="6" max="6" width="30.5" customWidth="1"/>
     <col min="7" max="8" width="31.33203125" customWidth="1"/>
     <col min="9" max="9" width="31.83203125" customWidth="1"/>
+    <col min="10" max="10" width="30.5" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -911,8 +953,14 @@
       <c r="I4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>0</v>
       </c>
@@ -937,8 +985,14 @@
       <c r="I5">
         <v>0.81565079365079296</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>0.91931746031745998</v>
+      </c>
+      <c r="K5">
+        <v>0.85133333333333305</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -963,8 +1017,14 @@
       <c r="I6">
         <v>0.87431746031746005</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0.94926984126984104</v>
+      </c>
+      <c r="K6">
+        <v>0.84688888888888803</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -989,8 +1049,14 @@
       <c r="I7">
         <v>0.91007936507936504</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0.96961904761904705</v>
+      </c>
+      <c r="K7">
+        <v>0.84588888888888802</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>3</v>
       </c>
@@ -1015,8 +1081,14 @@
       <c r="I8">
         <v>0.92312698412698402</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>0.98088888888888803</v>
+      </c>
+      <c r="K8">
+        <v>0.84599999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>4</v>
       </c>
@@ -1041,8 +1113,14 @@
       <c r="I9">
         <v>0.94266666666666599</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>0.98630158730158701</v>
+      </c>
+      <c r="K9">
+        <v>0.846444444444444</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>5</v>
       </c>
@@ -1067,8 +1145,14 @@
       <c r="I10">
         <v>0.95079365079364997</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>0.99047619047618995</v>
+      </c>
+      <c r="K10">
+        <v>0.84044444444444399</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>6</v>
       </c>
@@ -1093,8 +1177,14 @@
       <c r="I11">
         <v>0.949031746031746</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>0.99166666666666603</v>
+      </c>
+      <c r="K11">
+        <v>0.83855555555555505</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>7</v>
       </c>
@@ -1119,8 +1209,14 @@
       <c r="I12">
         <v>0.96077777777777695</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0.99296825396825295</v>
+      </c>
+      <c r="K12">
+        <v>0.83711111111111103</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>8</v>
       </c>
@@ -1145,8 +1241,14 @@
       <c r="I13">
         <v>0.96706349206349196</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>0.99631746031746005</v>
+      </c>
+      <c r="K13">
+        <v>0.84333333333333305</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>9</v>
       </c>
@@ -1170,6 +1272,12 @@
       </c>
       <c r="I14">
         <v>0.96949206349206296</v>
+      </c>
+      <c r="J14">
+        <v>0.99653968253968195</v>
+      </c>
+      <c r="K14">
+        <v>0.83911111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -1179,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81FE0B0-99D3-464F-8FF5-7416433A4FBB}">
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1196,15 +1304,19 @@
     <col min="7" max="7" width="31.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34" customWidth="1"/>
+    <col min="11" max="11" width="41.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -1229,8 +1341,20 @@
       <c r="I4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>0</v>
       </c>
@@ -1255,8 +1379,20 @@
       <c r="I5">
         <v>0.89107936507936503</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>0.87326984126984097</v>
+      </c>
+      <c r="K5">
+        <v>0.83355555555555505</v>
+      </c>
+      <c r="L5">
+        <v>0.91695238095238096</v>
+      </c>
+      <c r="M5">
+        <v>0.84866666666666601</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -1281,8 +1417,20 @@
       <c r="I6">
         <v>0.91857142857142804</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0.927539682539682</v>
+      </c>
+      <c r="K6">
+        <v>0.83911111111111103</v>
+      </c>
+      <c r="L6">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="M6">
+        <v>0.845444444444444</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -1307,8 +1455,20 @@
       <c r="I7">
         <v>0.93326984126984103</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0.96244444444444399</v>
+      </c>
+      <c r="K7">
+        <v>0.83533333333333304</v>
+      </c>
+      <c r="L7">
+        <v>0.97047619047619005</v>
+      </c>
+      <c r="M7">
+        <v>0.84566666666666601</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>3</v>
       </c>
@@ -1333,8 +1493,20 @@
       <c r="I8">
         <v>0.94420634920634905</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>0.97847619047619006</v>
+      </c>
+      <c r="K8">
+        <v>0.83422222222222198</v>
+      </c>
+      <c r="L8">
+        <v>0.98120634920634897</v>
+      </c>
+      <c r="M8">
+        <v>0.846444444444444</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>4</v>
       </c>
@@ -1359,8 +1531,20 @@
       <c r="I9">
         <v>0.94993650793650797</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>0.986507936507936</v>
+      </c>
+      <c r="K9">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="L9">
+        <v>0.98682539682539605</v>
+      </c>
+      <c r="M9">
+        <v>0.84233333333333305</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>5</v>
       </c>
@@ -1385,8 +1569,20 @@
       <c r="I10">
         <v>0.95242857142857096</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>0.98969841269841197</v>
+      </c>
+      <c r="K10">
+        <v>0.82522222222222197</v>
+      </c>
+      <c r="L10">
+        <v>0.990079365079365</v>
+      </c>
+      <c r="M10">
+        <v>0.842444444444444</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>6</v>
       </c>
@@ -1411,8 +1607,20 @@
       <c r="I11">
         <v>0.95587301587301499</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>0.99433333333333296</v>
+      </c>
+      <c r="K11">
+        <v>0.82788888888888801</v>
+      </c>
+      <c r="L11">
+        <v>0.99406349206349198</v>
+      </c>
+      <c r="M11">
+        <v>0.84266666666666601</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>7</v>
       </c>
@@ -1437,8 +1645,20 @@
       <c r="I12">
         <v>0.95630158730158699</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0.99676190476190396</v>
+      </c>
+      <c r="K12">
+        <v>0.82377777777777705</v>
+      </c>
+      <c r="L12">
+        <v>0.99553968253968195</v>
+      </c>
+      <c r="M12">
+        <v>0.84033333333333304</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>8</v>
       </c>
@@ -1463,8 +1683,20 @@
       <c r="I13">
         <v>0.95950793650793598</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>0.99798412698412697</v>
+      </c>
+      <c r="K13">
+        <v>0.82355555555555504</v>
+      </c>
+      <c r="L13">
+        <v>0.99461904761904696</v>
+      </c>
+      <c r="M13">
+        <v>0.837666666666666</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>9</v>
       </c>
@@ -1488,6 +1720,18 @@
       </c>
       <c r="I14">
         <v>0.96379365079364998</v>
+      </c>
+      <c r="J14">
+        <v>0.99860317460317405</v>
+      </c>
+      <c r="K14">
+        <v>0.82033333333333303</v>
+      </c>
+      <c r="L14">
+        <v>0.99669841269841197</v>
+      </c>
+      <c r="M14">
+        <v>0.83633333333333304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added assets 1. Added preprocessing example. 2. Modified hyperparameter comparison file.
</commit_message>
<xml_diff>
--- a/analysis/hyperparameters_comparison.xlsx
+++ b/analysis/hyperparameters_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandraastakhova/Projects/Python/Quick Draw/quick-draw-image-recognition/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2B8DFB-B214-AE46-B5CD-60E446049B0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D9FAC2-3DD9-7744-BB2C-3DCC08E19F7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="1600" windowWidth="28240" windowHeight="17560" activeTab="2" xr2:uid="{7776EE55-F732-E243-947B-1C2E89181C75}"/>
+    <workbookView xWindow="3120" yWindow="1760" windowWidth="28240" windowHeight="17560" activeTab="1" xr2:uid="{7776EE55-F732-E243-947B-1C2E89181C75}"/>
   </bookViews>
   <sheets>
     <sheet name="Original dataset" sheetId="1" r:id="rId1"/>
@@ -147,6 +147,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -185,15 +188,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFD541"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -203,6 +213,2631 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en"/>
+              <a:t>Basic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en" baseline="0"/>
+              <a:t> Neural Network</a:t>
+            </a:r>
+            <a:endParaRPr lang="en"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFD541"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFD541"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FFD541"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Original dataset'!$C$5:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Original dataset'!$D$5:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.82022222222222196</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79755555555555502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79911111111111099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80844444444444397</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81344444444444397</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81633333333333302</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.80822222222222195</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.818888888888888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81155555555555503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.81322222222222196</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-14A7-5347-8AFE-C170119BCCC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Train</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Original dataset'!$C$5:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Original dataset'!$E$5:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.87847619047618997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92838095238095197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.956238095238095</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97614285714285698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99909523809523804</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99990476190476096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99990476190476096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99990476190476096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99990476190476096</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99990476190476096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-14A7-5347-8AFE-C170119BCCC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="364315951"/>
+        <c:axId val="364243023"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="364315951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en"/>
+                  <a:t>Epochs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="364243023"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="364243023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.70000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en"/>
+                  <a:t>Accuracy,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en" baseline="0"/>
+                  <a:t> %</a:t>
+                </a:r>
+                <a:endParaRPr lang="en"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="364315951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Basic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Neural Network with Expanded Dataset</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFD541"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFD541"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FFD541"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Expanded dataset'!$C$5:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expanded dataset'!$D$5:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.82799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84733333333333305</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84355555555555495</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84211111111111103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82511111111111102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82822222222222197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82877777777777695</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.822888888888888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83277777777777695</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.832666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2802-5D46-8601-77B6E43D6317}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Train</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Expanded dataset'!$C$5:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expanded dataset'!$E$5:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.86199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93088888888888799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97466666666666602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98295238095238002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98668253968253905</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99574603174603105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96053968253968203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99995238095238004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99996825396825395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2802-5D46-8601-77B6E43D6317}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="229565263"/>
+        <c:axId val="360720543"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="229565263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en"/>
+                  <a:t>Epochs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="360720543"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="360720543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.70000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="229565263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47E0B36E-6A35-9342-BAAE-416CBA06F653}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>850900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BEC3A02-AA92-C641-AEBD-9EEEF9C1B00A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,7 +3156,7 @@
   <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,10 +3218,10 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.82022222222222196</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.87847619047618997</v>
       </c>
       <c r="F5">
@@ -615,10 +3250,10 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.79755555555555502</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0.92838095238095197</v>
       </c>
       <c r="F6">
@@ -647,10 +3282,10 @@
       <c r="C7">
         <v>30</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.79911111111111099</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.956238095238095</v>
       </c>
       <c r="F7">
@@ -679,10 +3314,10 @@
       <c r="C8">
         <v>40</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.80844444444444397</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>0.97614285714285698</v>
       </c>
       <c r="F8">
@@ -711,10 +3346,10 @@
       <c r="C9">
         <v>50</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.81344444444444397</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>0.99909523809523804</v>
       </c>
       <c r="F9">
@@ -743,10 +3378,10 @@
       <c r="C10">
         <v>60</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.81633333333333302</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>0.99990476190476096</v>
       </c>
       <c r="F10">
@@ -775,10 +3410,10 @@
       <c r="C11">
         <v>70</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.80822222222222195</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>0.99990476190476096</v>
       </c>
       <c r="F11">
@@ -807,10 +3442,10 @@
       <c r="C12">
         <v>80</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>0.818888888888888</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>0.99990476190476096</v>
       </c>
       <c r="F12">
@@ -839,10 +3474,10 @@
       <c r="C13">
         <v>90</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>0.81155555555555503</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>0.99990476190476096</v>
       </c>
       <c r="F13">
@@ -871,10 +3506,10 @@
       <c r="C14">
         <v>100</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0.81322222222222196</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>0.99990476190476096</v>
       </c>
       <c r="F14">
@@ -898,6 +3533,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -905,8 +3541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8339C909-F14C-2C4C-BA89-011C8338A229}">
   <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,10 +3603,10 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.82799999999999996</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.86199999999999999</v>
       </c>
       <c r="F5">
@@ -999,10 +3635,10 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.84733333333333305</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0.93088888888888799</v>
       </c>
       <c r="F6">
@@ -1031,10 +3667,10 @@
       <c r="C7">
         <v>30</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.84355555555555495</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.95499999999999996</v>
       </c>
       <c r="F7">
@@ -1063,10 +3699,10 @@
       <c r="C8">
         <v>40</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.84211111111111103</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>0.97466666666666602</v>
       </c>
       <c r="F8">
@@ -1095,10 +3731,10 @@
       <c r="C9">
         <v>50</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.82511111111111102</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>0.98295238095238002</v>
       </c>
       <c r="F9">
@@ -1127,10 +3763,10 @@
       <c r="C10">
         <v>60</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.82822222222222197</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>0.98668253968253905</v>
       </c>
       <c r="F10">
@@ -1159,10 +3795,10 @@
       <c r="C11">
         <v>70</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.82877777777777695</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>0.99574603174603105</v>
       </c>
       <c r="F11">
@@ -1191,10 +3827,10 @@
       <c r="C12">
         <v>80</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>0.822888888888888</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>0.96053968253968203</v>
       </c>
       <c r="F12">
@@ -1223,10 +3859,10 @@
       <c r="C13">
         <v>90</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>0.83277777777777695</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>0.99995238095238004</v>
       </c>
       <c r="F13">
@@ -1255,10 +3891,10 @@
       <c r="C14">
         <v>100</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0.832666666666666</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>0.99996825396825395</v>
       </c>
       <c r="F14">
@@ -1282,6 +3918,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1289,8 +3926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81FE0B0-99D3-464F-8FF5-7416433A4FBB}">
   <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finalized the project report and the model evaluation results: 1. Added model evaluation results to hyperparameter_comparison file. 2. Added project report 'Quick Draw Report.pdf'.
</commit_message>
<xml_diff>
--- a/analysis/hyperparameters_comparison.xlsx
+++ b/analysis/hyperparameters_comparison.xlsx
@@ -8,18 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandraastakhova/Projects/Python/Quick Draw/quick-draw-image-recognition/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D9FAC2-3DD9-7744-BB2C-3DCC08E19F7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1639F85C-148A-2543-9093-761C69CA20EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1760" windowWidth="28240" windowHeight="17560" activeTab="1" xr2:uid="{7776EE55-F732-E243-947B-1C2E89181C75}"/>
+    <workbookView xWindow="1860" yWindow="460" windowWidth="28240" windowHeight="17560" activeTab="3" xr2:uid="{7776EE55-F732-E243-947B-1C2E89181C75}"/>
   </bookViews>
   <sheets>
     <sheet name="Original dataset" sheetId="1" r:id="rId1"/>
     <sheet name="Expanded dataset" sheetId="2" r:id="rId2"/>
     <sheet name="Adam optimizer" sheetId="3" r:id="rId3"/>
+    <sheet name="More Epochs" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="comparison_1557179772.093524" localSheetId="2">'Adam optimizer'!$B$4:$I$14</definedName>
     <definedName name="hyperparameter_comparison" localSheetId="0">'Original dataset'!$B$4:$K$14</definedName>
+    <definedName name="learning_curve_1558725347.69086" localSheetId="3">'More Epochs'!$B$4:$D$24</definedName>
+    <definedName name="learning_curve_1558794019.59101" localSheetId="3">'More Epochs'!$E$4:$F$24</definedName>
     <definedName name="learning_curve_adam_batch_norm" localSheetId="2">'Adam optimizer'!$J$4:$K$14</definedName>
     <definedName name="learning_curve_adam_batch_norm_7000" localSheetId="2">'Adam optimizer'!$L$4:$M$14</definedName>
   </definedNames>
@@ -68,7 +71,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{271E221C-F4AB-E244-B1AF-B9CEDBEFB65D}" name="learning_curve_adam_batch_norm" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{9B5ABC7A-05D4-0E41-B4FB-0CF970C53DF6}" name="learning_curve_1558725347.69086" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10007" sourceFile="/Users/aleksandraastakhova/Projects/Python/Quick Draw/learning_curve_1558725347.69086.csv" thousands=" " tab="0" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" xr16:uid="{CE3E91E1-4939-B54E-B925-C6294B37B298}" name="learning_curve_1558794019.59101" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10007" sourceFile="/Users/aleksandraastakhova/Projects/Python/Quick Draw/learning_curve_1558794019.59101.csv" thousands=" " tab="0" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" xr16:uid="{271E221C-F4AB-E244-B1AF-B9CEDBEFB65D}" name="learning_curve_adam_batch_norm" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10007" sourceFile="/Users/aleksandraastakhova/Projects/Python/Quick Draw/learning_curve_adam_batch_norm.csv" thousands=" " tab="0" comma="1">
       <textFields count="3">
         <textField/>
@@ -77,7 +98,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{AD48D861-32E6-F54D-AEB1-B3E184D14A53}" name="learning_curve_adam_batch_norm_7000" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="6" xr16:uid="{AD48D861-32E6-F54D-AEB1-B3E184D14A53}" name="learning_curve_adam_batch_norm_7000" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10007" sourceFile="/Users/aleksandraastakhova/Projects/Python/Quick Draw/learning_curve_adam_batch_norm_7000.csv" thousands=" " tab="0" comma="1">
       <textFields count="3">
         <textField type="skip"/>
@@ -90,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>test weight_decay: 0.0, dropout: 0.0</t>
   </si>
@@ -142,15 +163,27 @@
   <si>
     <t>test batch norm weight_decay: 0.0, dropout: 0.0, mini batches = 7000</t>
   </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Dropout = 0.3, weght decay = 0, learning rate = 0.03, minibatches = 7000, optimizer = Adam</t>
+  </si>
+  <si>
+    <t>Dropout = 0.5, weght decay = 0, learning rate = 0.03, minibatches = 7000, optimizer = Adam</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +198,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -185,17 +226,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1672,6 +1716,1130 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en"/>
+              <a:t> Basic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en" baseline="0"/>
+              <a:t> Neural Network with Regularization</a:t>
+            </a:r>
+            <a:endParaRPr lang="en"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Epochs'!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Dropout = 0.3, weght decay = 0, learning rate = 0.03, minibatches = 7000, optimizer = Adam</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'More Epochs'!$B$5:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Epochs'!$C$5:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.88958730158730104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92455555555555502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94042857142857095</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95185714285714196</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96263492063491995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96688888888888802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97153968253968204</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97563492063491997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.976301587301587</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97903174603174603</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98001587301587301</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98401587301587301</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98617460317460304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98638095238095203</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98588888888888804</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98815873015873001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98941269841269797</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98985714285714199</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99114285714285699</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99068253968253905</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B7C5-EA40-AEFA-34E9E7AEA300}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Epochs'!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Dropout = 0.3, weght decay = 0, learning rate = 0.03, minibatches = 7000, optimizer = Adam</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'More Epochs'!$B$5:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Epochs'!$D$5:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.83333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85122222222222199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84077777777777696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83311111111111102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82844444444444398</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83455555555555505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82755555555555504</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83133333333333304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82944444444444398</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.82344444444444398</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83133333333333304</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82566666666666599</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.82855555555555505</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.82844444444444398</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.82855555555555505</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.82911111111111102</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.82244444444444398</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.82488888888888801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B7C5-EA40-AEFA-34E9E7AEA300}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Epochs'!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Dropout = 0.5, weght decay = 0, learning rate = 0.03, minibatches = 7000, optimizer = Adam</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'More Epochs'!$B$5:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Epochs'!$E$5:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.87226984126984097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90882539682539598</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92377777777777703</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93755555555555503</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94431746031746</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95057142857142796</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95376190476190403</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96261904761904704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96446031746031702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96739682539682503</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97034920634920596</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97366666666666601</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97514285714285698</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97758730158730101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.97887301587301501</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98082539682539605</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98158730158730101</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98292063492063497</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98342857142857099</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.98387301587301501</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B7C5-EA40-AEFA-34E9E7AEA300}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Epochs'!$F$3:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Dropout = 0.5, weght decay = 0, learning rate = 0.03, minibatches = 7000, optimizer = Adam</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFD541"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FFD541"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'More Epochs'!$B$5:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Epochs'!$F$5:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.82855555555555505</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83677777777777695</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83877777777777696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.836666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82788888888888801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82977777777777695</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.827666666666666</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.830666666666666</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.82311111111111102</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82811111111111102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.82422222222222197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.82488888888888801</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82155555555555504</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.830666666666666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.82122222222222196</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.820888888888888</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.82077777777777705</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.82422222222222197</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.82044444444444398</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.82011111111111101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B7C5-EA40-AEFA-34E9E7AEA300}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="155417327"/>
+        <c:axId val="121285599"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="155417327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en"/>
+                  <a:t>Epochs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="121285599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="121285599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.75000000000000011"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="155417327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1752,6 +2920,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2256,6 +3464,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2840,20 +4551,69 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7046DA10-EBD5-2E4D-9C9C-41DFBB0BB2DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hyperparameter_comparison" connectionId="2" xr16:uid="{BA1644FB-2D55-3E41-9BFC-E3B5AE7525F5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="learning_curve_adam_batch_norm_7000" connectionId="4" xr16:uid="{17E34221-FBAE-184A-930B-412F0C2EF5F0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="learning_curve_adam_batch_norm" connectionId="5" xr16:uid="{B3314429-B1B6-BE45-AB91-D2B05C6A27EF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="learning_curve_adam_batch_norm_7000" connectionId="6" xr16:uid="{17E34221-FBAE-184A-930B-412F0C2EF5F0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="comparison_1557179772.093524" connectionId="1" xr16:uid="{3BE52358-A770-7945-B8C3-771A99E8AA11}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="learning_curve_adam_batch_norm" connectionId="3" xr16:uid="{B3314429-B1B6-BE45-AB91-D2B05C6A27EF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="learning_curve_1558794019.59101" connectionId="4" xr16:uid="{1518C538-4CD9-474E-B612-8350208C91C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="learning_curve_1558725347.69086" connectionId="3" xr16:uid="{039CF50D-F58A-8945-9EE4-10E54CF11200}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3541,8 +5301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8339C909-F14C-2C4C-BA89-011C8338A229}">
   <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3927,7 +5687,7 @@
   <dimension ref="B2:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4374,4 +6134,390 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEAB7C3-3F93-4A41-9CA7-ADB06CBA0BE4}">
+  <dimension ref="B3:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="42.5" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.88958730158730104</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.87226984126984097</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.82855555555555505</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.92455555555555502</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.85122222222222199</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.90882539682539598</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.83677777777777695</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.94042857142857095</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.84077777777777696</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.92377777777777703</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.83877777777777696</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.95185714285714196</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.83311111111111102</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.93755555555555503</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.836666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.96263492063491995</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.82844444444444398</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.94431746031746</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.82788888888888801</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.96688888888888802</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.83455555555555505</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.95057142857142796</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.82977777777777695</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>70</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.97153968253968204</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.82755555555555504</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.95376190476190403</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.827666666666666</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>80</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.97563492063491997</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.96261904761904704</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.830666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>90</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.976301587301587</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.83133333333333304</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.96446031746031702</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.82311111111111102</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.97903174603174603</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.82944444444444398</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.96739682539682503</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.82811111111111102</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>110</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.98001587301587301</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.82344444444444398</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.97034920634920596</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.82422222222222197</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>120</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.98401587301587301</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.83133333333333304</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.97366666666666601</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.82488888888888801</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>130</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.98617460317460304</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.82566666666666599</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.97514285714285698</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.82155555555555504</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>140</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.98638095238095203</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.82855555555555505</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.97758730158730101</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.830666666666666</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>150</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.98588888888888804</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.82844444444444398</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.97887301587301501</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.82122222222222196</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>160</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.98815873015873001</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.82855555555555505</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.98082539682539605</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.820888888888888</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>170</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.98941269841269797</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.82911111111111102</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.98158730158730101</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.82077777777777705</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>180</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.98985714285714199</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.82</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.98292063492063497</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.82422222222222197</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>190</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.99114285714285699</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.82244444444444398</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.98342857142857099</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.82044444444444398</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>200</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.99068253968253905</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.82488888888888801</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.98387301587301501</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.82011111111111101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>